<commit_message>
Standup meeting added to daily standup document
</commit_message>
<xml_diff>
--- a/Documents/Daily standup meetings.xlsx
+++ b/Documents/Daily standup meetings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
   <si>
     <t>Daily standup meeting 15/02/2016:</t>
   </si>
@@ -79,6 +79,51 @@
   </si>
   <si>
     <t>Iedereen aanwezig</t>
+  </si>
+  <si>
+    <t>Knights Tour</t>
+  </si>
+  <si>
+    <t>Knights Tour document en uploaden</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>problemen met ogre, hulp nodig</t>
+  </si>
+  <si>
+    <t>Knights Tour beginnen</t>
+  </si>
+  <si>
+    <t>Cannot find path issue</t>
+  </si>
+  <si>
+    <t>3d modellen uitgebreid. Ogre werkend</t>
+  </si>
+  <si>
+    <t>Knights Tour afmaken en document</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Veel zeldzame errors met visual studio</t>
+  </si>
+  <si>
+    <t>bugfixing ogre</t>
+  </si>
+  <si>
+    <t>Ogre fixen</t>
+  </si>
+  <si>
+    <t>Ogre werkt in d9</t>
+  </si>
+  <si>
+    <t>Directx11 werkt niet met runnen</t>
+  </si>
+  <si>
+    <t>Knights tour afronden</t>
   </si>
 </sst>
 </file>
@@ -460,13 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -476,7 +523,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -486,7 +533,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
@@ -505,7 +552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -519,7 +566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -533,7 +580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -547,7 +594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -561,7 +608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -575,7 +622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -585,7 +632,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -595,7 +642,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D12" s="5" t="s">
         <v>3</v>
       </c>
@@ -610,6 +657,261 @@
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
+      <c r="Q12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
       <c r="O12" s="5" t="s">
         <v>8</v>
       </c>
@@ -618,70 +920,25 @@
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" t="s">
-        <v>15</v>
-      </c>
-      <c r="O13" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L14" t="s">
-        <v>15</v>
-      </c>
-      <c r="O14" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" t="s">
-        <v>15</v>
-      </c>
-      <c r="O15" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" t="s">
-        <v>15</v>
-      </c>
-      <c r="O16" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17" t="s">
-        <v>9</v>
-      </c>
-      <c r="O17" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
@@ -727,86 +984,156 @@
       <c r="A22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="L22" t="s">
-        <v>15</v>
-      </c>
-      <c r="O22" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" t="s">
-        <v>15</v>
-      </c>
-      <c r="O23" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="L24" t="s">
-        <v>15</v>
-      </c>
-      <c r="O24" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L25" t="s">
-        <v>15</v>
-      </c>
-      <c r="O25" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="L26" t="s">
-        <v>9</v>
-      </c>
-      <c r="O26" t="s">
-        <v>9</v>
+    </row>
+    <row r="28" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>